<commit_message>
added test for read holdings
</commit_message>
<xml_diff>
--- a/samples/holding _ 16032017.xlsx
+++ b/samples/holding _ 16032017.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuta\git\cmbhk\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C415BA-A4BA-4D1A-B9E1-A1FFFB46A562}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="3135" windowWidth="21840" windowHeight="11985"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Client Name</t>
   </si>
@@ -356,15 +370,19 @@
     <t>USD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Corrupt Header</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -470,17 +488,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -498,10 +516,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -510,13 +528,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -528,7 +546,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -537,26 +555,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="2"/>
-    <cellStyle name="常规 2 2" xfId="4"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="千位分隔 2" xfId="3"/>
-    <cellStyle name="千位分隔 3" xfId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="千位分隔 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -579,7 +600,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 8" descr="CMB%20Logo4"/>
+        <xdr:cNvPr id="2" name="图片 8" descr="CMB%20Logo4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -623,7 +650,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,7 +692,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,9 +725,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,6 +777,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -908,38 +969,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:J20"/>
+  <dimension ref="A4:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1328125" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,7 +1014,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -967,7 +1028,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12" ht="15">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -981,7 +1042,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="13"/>
       <c r="C8" s="8"/>
@@ -991,7 +1052,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" ht="40.5">
+    <row r="9" spans="1:12" s="12" customFormat="1" ht="38.65">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
@@ -1022,8 +1083,11 @@
       <c r="J9" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1121,7 @@
         <v>19134615.384615384</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:12">
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
@@ -1091,7 +1155,7 @@
         <v>510256.41025641025</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
@@ -1125,7 +1189,7 @@
         <v>1635897.435897436</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:12">
       <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
@@ -1159,7 +1223,7 @@
         <v>100974358.97435898</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:12">
       <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
@@ -1193,7 +1257,7 @@
         <v>3724358.974358974</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:12">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -1227,7 +1291,7 @@
         <v>56307692.307692312</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:12">
       <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
@@ -1393,7 +1457,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A11:H52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:H52">
     <sortCondition ref="B11:B52"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1404,7 +1468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1417,7 +1481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1426,5 +1490,6 @@
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>